<commit_message>
Insertar descuento para cada cliente en el archivo Excel
</commit_message>
<xml_diff>
--- a/facturas/Invoice 1.xlsx
+++ b/facturas/Invoice 1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bianca.dragu\Documents\03. RPA Starter\Build Your First Automation\Invoices - Working Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0642ad1663edb63c/Documents/UiPath/DescuentosFacturas/facturas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69BB415E-CF17-4EFC-9354-AFE2B9AEF6CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{69BB415E-CF17-4EFC-9354-AFE2B9AEF6CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0D0C0362-D0A7-40AE-86D8-0BDB92ACB9E0}"/>
   <bookViews>
-    <workbookView xWindow="15912" yWindow="-15900" windowWidth="12984" windowHeight="12612" xr2:uid="{ACCB1FA6-7E67-4590-BB25-A17FCE65C786}"/>
+    <workbookView xWindow="4545" yWindow="1875" windowWidth="15375" windowHeight="9000" xr2:uid="{ACCB1FA6-7E67-4590-BB25-A17FCE65C786}"/>
   </bookViews>
   <sheets>
     <sheet name="Invoice" sheetId="1" r:id="rId1"/>
@@ -123,7 +123,7 @@
     <t>CLIENT CODE</t>
   </si>
   <si>
-    <t>name, email address</t>
+    <t>RPA Developer - RPADeveloper@Uipath.com</t>
   </si>
 </sst>
 </file>
@@ -131,10 +131,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
-    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="0.000%"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="167" formatCode="0.000%"/>
   </numFmts>
   <fonts count="16" x14ac:knownFonts="1">
     <font>
@@ -416,9 +416,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
@@ -457,23 +456,23 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="6" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="6" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="6" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="44" fontId="8" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="8" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -485,24 +484,24 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="6" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="43" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="6" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="166" fontId="6" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -533,13 +532,25 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
@@ -552,21 +563,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -583,7 +582,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -885,384 +884,384 @@
       <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.54296875" customWidth="1"/>
-    <col min="3" max="3" width="19.453125" customWidth="1"/>
-    <col min="4" max="4" width="4.54296875" customWidth="1"/>
-    <col min="5" max="5" width="17.453125" customWidth="1"/>
-    <col min="6" max="6" width="21.08984375" customWidth="1"/>
-    <col min="7" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="9.140625" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" customWidth="1"/>
+    <col min="4" max="4" width="4.5703125" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" customWidth="1"/>
+    <col min="6" max="6" width="21.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="46" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:6" ht="46.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="43" t="s">
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="43"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="5" t="s">
+      <c r="F1" s="46"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="5" t="s">
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="5" t="s">
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="44" t="s">
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="E4" s="44"/>
-      <c r="F4" s="10" t="s">
+      <c r="E4" s="47"/>
+      <c r="F4" s="9" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4">
         <v>2034</v>
       </c>
-      <c r="F5" s="11">
+      <c r="F5" s="10">
         <v>44329</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="8"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="47" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="48"/>
-      <c r="C7" s="40"/>
-      <c r="D7" s="44" t="s">
+      <c r="B7" s="43"/>
+      <c r="C7" s="39"/>
+      <c r="D7" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="44"/>
-      <c r="F7" s="10" t="s">
+      <c r="E7" s="47"/>
+      <c r="F7" s="9" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" s="8" t="s">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="37"/>
-      <c r="E8" s="37">
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="36"/>
+      <c r="E8" s="36">
         <v>564</v>
       </c>
-      <c r="F8" s="13" t="s">
+      <c r="F8" s="12" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" s="8" t="s">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10" s="8" t="s">
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" s="8" t="s">
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" s="8" t="s">
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" s="14" t="s">
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14" s="8"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15" s="23" t="s">
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="7"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="23"/>
-      <c r="C15" s="39"/>
-      <c r="D15" s="24" t="s">
+      <c r="B15" s="22"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="E15" s="24" t="s">
+      <c r="E15" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="F15" s="24" t="s">
+      <c r="F15" s="23" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="35" t="s">
+    <row r="16" spans="1:6" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="35"/>
-      <c r="C16" s="35"/>
-      <c r="D16" s="31">
+      <c r="B16" s="34"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="30">
         <v>1</v>
       </c>
-      <c r="E16" s="26">
+      <c r="E16" s="25">
         <v>200</v>
       </c>
-      <c r="F16" s="27">
+      <c r="F16" s="26">
         <f>IF(D16="",ROUND(1*E16,2),ROUND(D16*E16,2))</f>
         <v>200</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="36" t="s">
+    <row r="17" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="36"/>
-      <c r="C17" s="36"/>
-      <c r="D17" s="32">
+      <c r="B17" s="35"/>
+      <c r="C17" s="35"/>
+      <c r="D17" s="31">
         <v>5</v>
       </c>
-      <c r="E17" s="28">
+      <c r="E17" s="27">
         <v>175</v>
       </c>
-      <c r="F17" s="29">
+      <c r="F17" s="28">
         <f t="shared" ref="F17:F20" si="0">IF(D17="",ROUND(1*E17,2),ROUND(D17*E17,2))</f>
         <v>875</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="20.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="36" t="s">
+    <row r="18" spans="1:6" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="36"/>
-      <c r="C18" s="36"/>
-      <c r="D18" s="32"/>
-      <c r="E18" s="30">
-        <v>1</v>
-      </c>
-      <c r="F18" s="29">
+      <c r="B18" s="35"/>
+      <c r="C18" s="35"/>
+      <c r="D18" s="31"/>
+      <c r="E18" s="29">
+        <v>100</v>
+      </c>
+      <c r="F18" s="28">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A19" s="36"/>
-      <c r="B19" s="36"/>
-      <c r="C19" s="36"/>
-      <c r="D19" s="33"/>
-      <c r="E19" s="28"/>
-      <c r="F19" s="29">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="35"/>
+      <c r="B19" s="35"/>
+      <c r="C19" s="35"/>
+      <c r="D19" s="32"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A20" s="34"/>
-      <c r="B20" s="34"/>
-      <c r="C20" s="34"/>
-      <c r="D20" s="32"/>
-      <c r="E20" s="28"/>
-      <c r="F20" s="29">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="33"/>
+      <c r="B20" s="33"/>
+      <c r="C20" s="33"/>
+      <c r="D20" s="31"/>
+      <c r="E20" s="27"/>
+      <c r="F20" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A21" s="45" t="s">
+    <row r="21" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="B21" s="45"/>
-      <c r="C21" s="45"/>
-      <c r="D21" s="46" t="s">
+      <c r="B21" s="40"/>
+      <c r="C21" s="40"/>
+      <c r="D21" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="E21" s="46"/>
-      <c r="F21" s="25">
+      <c r="E21" s="41"/>
+      <c r="F21" s="24">
         <f>SUM(F16:F20)</f>
-        <v>1076</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A22" s="16"/>
-      <c r="B22" s="17"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="41" t="s">
+        <v>1175</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="15"/>
+      <c r="B22" s="16"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="E22" s="41"/>
-      <c r="F22" s="18">
+      <c r="E22" s="44"/>
+      <c r="F22" s="17">
         <v>4.2500000000000003E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A23" s="16"/>
-      <c r="B23" s="17"/>
-      <c r="C23" s="17"/>
-      <c r="D23" s="19" t="s">
+    <row r="23" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="15"/>
+      <c r="B23" s="16"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="E23" s="19"/>
-      <c r="F23" s="15">
+      <c r="E23" s="18"/>
+      <c r="F23" s="14">
         <f>F21*F22</f>
-        <v>45.730000000000004</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="A24" s="16"/>
-      <c r="B24" s="17"/>
-      <c r="C24" s="17"/>
-      <c r="D24" s="42" t="s">
+        <v>49.937500000000007</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="15"/>
+      <c r="B24" s="16"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="E24" s="42"/>
-      <c r="F24" s="20">
+      <c r="E24" s="45"/>
+      <c r="F24" s="19">
         <f>F21+F23</f>
-        <v>1121.73</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A25" s="7"/>
-      <c r="B25" s="12"/>
-      <c r="C25" s="12"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="21"/>
-      <c r="F25" s="21"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A26" s="12"/>
-      <c r="B26" s="12"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A27" s="22"/>
-      <c r="B27" s="22"/>
-      <c r="C27" s="22"/>
-      <c r="D27" s="22"/>
-      <c r="E27" s="22"/>
-      <c r="F27" s="22"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A28" s="22"/>
-      <c r="B28" s="22"/>
-      <c r="C28" s="22"/>
-      <c r="D28" s="22"/>
-      <c r="E28" s="22"/>
-      <c r="F28" s="22"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A29" s="22"/>
-      <c r="B29" s="22"/>
-      <c r="C29" s="22"/>
-      <c r="D29" s="22"/>
-      <c r="E29" s="22"/>
-      <c r="F29" s="22"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A30" s="22"/>
-      <c r="B30" s="22"/>
-      <c r="C30" s="22"/>
-      <c r="D30" s="22"/>
-      <c r="E30" s="22"/>
-      <c r="F30" s="22"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A31" s="38" t="s">
+        <v>1224.9375</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="6"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="11"/>
+      <c r="B26" s="11"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="11"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="21"/>
+      <c r="B27" s="21"/>
+      <c r="C27" s="21"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="21"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="21"/>
+      <c r="B28" s="21"/>
+      <c r="C28" s="21"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="21"/>
+      <c r="F28" s="21"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="21"/>
+      <c r="B29" s="21"/>
+      <c r="C29" s="21"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="21"/>
+      <c r="F29" s="21"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="21"/>
+      <c r="B30" s="21"/>
+      <c r="C30" s="21"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="21"/>
+      <c r="F30" s="21"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="B31" s="38"/>
-      <c r="C31" s="38"/>
-      <c r="D31" s="38"/>
-      <c r="E31" s="38"/>
-      <c r="F31" s="38"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A32" s="9"/>
-      <c r="B32" s="9"/>
-      <c r="C32" s="9"/>
-      <c r="D32" s="9"/>
-      <c r="E32" s="9"/>
-      <c r="F32" s="9"/>
+      <c r="B31" s="37"/>
+      <c r="C31" s="37"/>
+      <c r="D31" s="37"/>
+      <c r="E31" s="37"/>
+      <c r="F31" s="37"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="8"/>
+      <c r="B32" s="8"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="8"/>
+      <c r="E32" s="8"/>
+      <c r="F32" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D7:E7"/>
     <mergeCell ref="A21:C21"/>
     <mergeCell ref="D21:E21"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="D22:E22"/>
     <mergeCell ref="D24:E24"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D7:E7"/>
   </mergeCells>
   <dataValidations disablePrompts="1" count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1" xr:uid="{3973258D-70B0-4F2B-9A52-AA2F46F0125B}">

</xml_diff>

<commit_message>
Comprobar descuentos aplicables y crear borrador de correo con facturas procesadas
</commit_message>
<xml_diff>
--- a/facturas/Invoice 1.xlsx
+++ b/facturas/Invoice 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0642ad1663edb63c/Documents/UiPath/DescuentosFacturas/facturas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{69BB415E-CF17-4EFC-9354-AFE2B9AEF6CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0D0C0362-D0A7-40AE-86D8-0BDB92ACB9E0}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{69BB415E-CF17-4EFC-9354-AFE2B9AEF6CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2920FB84-3BB6-4A62-A128-B9BDB0000823}"/>
   <bookViews>
     <workbookView xWindow="4545" yWindow="1875" windowWidth="15375" windowHeight="9000" xr2:uid="{ACCB1FA6-7E67-4590-BB25-A17FCE65C786}"/>
   </bookViews>
@@ -123,7 +123,7 @@
     <t>CLIENT CODE</t>
   </si>
   <si>
-    <t>RPA Developer - RPADeveloper@Uipath.com</t>
+    <t>RPA Developer - RPADeveloper@uipath.com</t>
   </si>
 </sst>
 </file>
@@ -880,7 +880,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A97115AB-6036-460D-B2FF-77BC506C7ACA}">
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
       <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>

</xml_diff>